<commit_message>
[DM] [add field] scinario_10
</commit_message>
<xml_diff>
--- a/app/seeds/item.xlsx
+++ b/app/seeds/item.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="102">
   <si>
     <t>名前</t>
   </si>
@@ -486,6 +486,10 @@
   </si>
   <si>
     <t>くさりかたびら</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>skill_cd</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -580,8 +584,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3977">
+  <cellStyleXfs count="3981">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4570,7 +4578,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3977">
+  <cellStyles count="3981">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -6559,6 +6567,8 @@
     <cellStyle name="ハイパーリンク" xfId="3971" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3973" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3975" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="3977" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="3979" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -8548,6 +8558,8 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="3972" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="3974" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="3976" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="3978" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="3980" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -8881,10 +8893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -9061,256 +9073,271 @@
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="5"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="A16" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:8">
+      <c r="A17" s="5"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:8">
+      <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="H19" s="3" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="2">
+    <row r="20" spans="1:8">
+      <c r="A20" s="2">
         <v>10001</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B20" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C20" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D20" s="8">
         <v>2</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="2">
-        <v>10002</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="8">
-        <v>4</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
+      <c r="H20" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="A21" s="2">
-        <v>10003</v>
+        <v>10002</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D21" s="8">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
+      <c r="H21" s="2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="A22" s="2">
-        <v>10004</v>
+        <v>10003</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D22" s="8">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
+      <c r="H22" s="2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8">
       <c r="A23" s="2">
-        <v>10005</v>
+        <v>10004</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D23" s="8">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:8">
       <c r="A24" s="2">
-        <v>10006</v>
+        <v>10005</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D24" s="8">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:8">
       <c r="A25" s="2">
-        <v>10007</v>
+        <v>10006</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D25" s="8">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2" t="b">
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="2">
+        <v>10007</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="8">
+        <v>40</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="H26" s="2"/>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="2">
+    <row r="27" spans="1:8">
+      <c r="A27" s="2">
         <v>10008</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B27" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="8">
-        <v>2</v>
-      </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="2">
-        <v>10009</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F27" s="8"/>
-      <c r="G27" s="2"/>
+      <c r="G27" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:8">
       <c r="A28" s="2">
-        <v>10010</v>
+        <v>10009</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="8">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:8">
       <c r="A29" s="2">
-        <v>10011</v>
+        <v>10010</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="8">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8">
       <c r="A30" s="2">
-        <v>10012</v>
+        <v>10011</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="8">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F30" s="8"/>
-      <c r="G30" s="2" t="s">
-        <v>87</v>
-      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:8">
       <c r="A31" s="2">
-        <v>10013</v>
+        <v>10012</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>83</v>
@@ -9320,130 +9347,158 @@
         <v>24</v>
       </c>
       <c r="F31" s="8"/>
-      <c r="G31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:8">
       <c r="A32" s="2">
-        <v>10014</v>
+        <v>10013</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="8">
-        <v>28</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>91</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:8">
       <c r="A33" s="2">
-        <v>10015</v>
+        <v>10014</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="8">
-        <v>4</v>
-      </c>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:8">
       <c r="A34" s="2">
-        <v>10016</v>
+        <v>10015</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>93</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="8">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:8">
       <c r="A35" s="2">
-        <v>10017</v>
+        <v>10016</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>93</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:8">
       <c r="A36" s="2">
-        <v>10018</v>
+        <v>10017</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="8">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:8">
       <c r="A37" s="2">
-        <v>10019</v>
+        <v>10018</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>97</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:8">
       <c r="A38" s="2">
-        <v>10020</v>
+        <v>10019</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>97</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="8">
+        <v>5</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="2">
+        <v>10020</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="8">
         <v>10</v>
       </c>
-      <c r="F38" s="8"/>
-      <c r="G38" s="2"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
[DM] [edit field] scinario_11
</commit_message>
<xml_diff>
--- a/app/seeds/item.xlsx
+++ b/app/seeds/item.xlsx
@@ -8896,7 +8896,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -9080,7 +9080,9 @@
         <v>13</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
       <c r="E16" s="3" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
[DM] [delete field] scinario_12
</commit_message>
<xml_diff>
--- a/app/seeds/item.xlsx
+++ b/app/seeds/item.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="101">
   <si>
     <t>名前</t>
   </si>
@@ -486,10 +486,6 @@
   </si>
   <si>
     <t>くさりかたびら</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>skill_cd</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -8893,10 +8889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18:H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -9073,273 +9069,256 @@
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="5"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2">
+        <v>10001</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="8">
+        <v>2</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:7">
       <c r="A20" s="2">
-        <v>10001</v>
+        <v>10002</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D20" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="2">
-        <v>1</v>
-      </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:7">
       <c r="A21" s="2">
-        <v>10002</v>
+        <v>10003</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D21" s="8">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2">
-        <v>2</v>
-      </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:7">
       <c r="A22" s="2">
-        <v>10003</v>
+        <v>10004</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D22" s="8">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="2">
-        <v>3</v>
-      </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:7">
       <c r="A23" s="2">
-        <v>10004</v>
+        <v>10005</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D23" s="8">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:7">
       <c r="A24" s="2">
-        <v>10005</v>
+        <v>10006</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D24" s="8">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:7">
       <c r="A25" s="2">
-        <v>10006</v>
+        <v>10007</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D25" s="8">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="G25" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:7">
       <c r="A26" s="2">
-        <v>10007</v>
+        <v>10008</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" s="8">
-        <v>40</v>
-      </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="2"/>
+        <v>83</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="8">
+        <v>2</v>
+      </c>
+      <c r="F26" s="8"/>
       <c r="G26" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H26" s="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:7">
       <c r="A27" s="2">
-        <v>10008</v>
+        <v>10009</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F27" s="8"/>
-      <c r="G27" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H27" s="2"/>
+      <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:7">
       <c r="A28" s="2">
-        <v>10009</v>
+        <v>10010</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="8">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:7">
       <c r="A29" s="2">
-        <v>10010</v>
+        <v>10011</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="8">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:7">
       <c r="A30" s="2">
-        <v>10011</v>
+        <v>10012</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="8">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F30" s="8"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="G30" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:7">
       <c r="A31" s="2">
-        <v>10012</v>
+        <v>10013</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>83</v>
@@ -9349,158 +9328,130 @@
         <v>24</v>
       </c>
       <c r="F31" s="8"/>
-      <c r="G31" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H31" s="2"/>
+      <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:7">
       <c r="A32" s="2">
-        <v>10013</v>
+        <v>10014</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="8">
-        <v>24</v>
-      </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:7">
       <c r="A33" s="2">
-        <v>10014</v>
+        <v>10015</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="8">
-        <v>28</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H33" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:7">
       <c r="A34" s="2">
-        <v>10015</v>
+        <v>10016</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>93</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="8">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:7">
       <c r="A35" s="2">
-        <v>10016</v>
+        <v>10017</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>93</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:7">
       <c r="A36" s="2">
-        <v>10017</v>
+        <v>10018</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="8">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:7">
       <c r="A37" s="2">
-        <v>10018</v>
+        <v>10019</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>97</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:7">
       <c r="A38" s="2">
-        <v>10019</v>
+        <v>10020</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>97</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="8">
-        <v>5</v>
-      </c>
-      <c r="F38" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="F38" s="8"/>
       <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="2">
-        <v>10020</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="8">
-        <v>10</v>
-      </c>
-      <c r="F39" s="8"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
[DM] [add data] scinario_13
</commit_message>
<xml_diff>
--- a/app/seeds/item.xlsx
+++ b/app/seeds/item.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="102">
   <si>
     <t>名前</t>
   </si>
@@ -486,6 +486,16 @@
   </si>
   <si>
     <t>くさりかたびら</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>金の兜</t>
+    <rPh sb="0" eb="1">
+      <t>キンオ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カブト</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -580,8 +590,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3981">
+  <cellStyleXfs count="3985">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4574,7 +4588,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3981">
+  <cellStyles count="3985">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -6565,6 +6579,8 @@
     <cellStyle name="ハイパーリンク" xfId="3975" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3977" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3979" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="3981" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="3983" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -8556,6 +8572,8 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="3976" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="3978" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="3980" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="3982" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="3984" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -8889,10 +8907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18:H38"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -9452,6 +9470,23 @@
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="2">
+        <v>10021</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="8">
+        <v>100</v>
+      </c>
+      <c r="F39" s="8"/>
+      <c r="G39" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
[DM] [edit data] scinario_14
</commit_message>
<xml_diff>
--- a/app/seeds/item.xlsx
+++ b/app/seeds/item.xlsx
@@ -489,11 +489,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>金の兜</t>
-    <rPh sb="0" eb="1">
-      <t>キンオ</t>
+    <t>黄金の兜</t>
+    <rPh sb="0" eb="2">
+      <t>オウゴン</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh sb="3" eb="4">
       <t>カブト</t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -8910,7 +8910,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
[DM] [delete data] scinario_15
</commit_message>
<xml_diff>
--- a/app/seeds/item.xlsx
+++ b/app/seeds/item.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="101">
   <si>
     <t>名前</t>
   </si>
@@ -486,16 +486,6 @@
   </si>
   <si>
     <t>くさりかたびら</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>黄金の兜</t>
-    <rPh sb="0" eb="2">
-      <t>オウゴン</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>カブト</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -8907,10 +8897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -9470,23 +9460,6 @@
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="2">
-        <v>10021</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="8">
-        <v>100</v>
-      </c>
-      <c r="F39" s="8"/>
-      <c r="G39" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>